<commit_message>
Generated the file for CustomerAbiomed, Inc - HQ @ Danvers, MA in the production server
</commit_message>
<xml_diff>
--- a/Abiomed, Inc - HQ @ Danvers, MA.xlsx
+++ b/Abiomed, Inc - HQ @ Danvers, MA.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Network Device" sheetId="1" r:id="rId1"/>
+    <sheet name="Server" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="121">
   <si>
     <t>Abiomed, Inc - HQ @ Danvers, MA</t>
   </si>
@@ -194,6 +195,189 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>ACAPT1-APZFS001</t>
+  </si>
+  <si>
+    <t>10.104.9.131</t>
+  </si>
+  <si>
+    <t>ACAPT1-WPPRN001</t>
+  </si>
+  <si>
+    <t>m5.xlarge</t>
+  </si>
+  <si>
+    <t>10.104.8.90</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2019 Datacenter  10.0.17763 Build 17763.3406</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.50GHz</t>
+  </si>
+  <si>
+    <t>ACAPT1-WPUTL002</t>
+  </si>
+  <si>
+    <t>10.104.8.175</t>
+  </si>
+  <si>
+    <t>ACAPT1-WPZDC001</t>
+  </si>
+  <si>
+    <t>m5.large</t>
+  </si>
+  <si>
+    <t>10.104.8.253</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2022 Datacenter  10.0.20348 Build 20348.768</t>
+  </si>
+  <si>
+    <t>ACAPT1-WPZDC002</t>
+  </si>
+  <si>
+    <t>10.104.9.116</t>
+  </si>
+  <si>
+    <t>ACAPT1-WPZDH001</t>
+  </si>
+  <si>
+    <t>10.104.8.157</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2022 Datacenter  10.0.20348 Build 20348.887</t>
+  </si>
+  <si>
+    <t>ACAPT1-WPZDH002</t>
+  </si>
+  <si>
+    <t>10.104.9.34</t>
+  </si>
+  <si>
+    <t>ACAPT1-WPZEM001</t>
+  </si>
+  <si>
+    <t>10.104.9.53</t>
+  </si>
+  <si>
+    <t>AUE1PRDAP01</t>
+  </si>
+  <si>
+    <t>t3.2xlarge</t>
+  </si>
+  <si>
+    <t>10.210.0.101</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2019 Datacenter  10.0.17763 Build 17763.3650</t>
+  </si>
+  <si>
+    <t>AUE1PRDAP02</t>
+  </si>
+  <si>
+    <t>10.210.1.101</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2019 Datacenter 10.0.17763 Build 17763.3650</t>
+  </si>
+  <si>
+    <t>AUE1PRDIN01</t>
+  </si>
+  <si>
+    <t>t3.xlarge</t>
+  </si>
+  <si>
+    <t>10.210.0.111</t>
+  </si>
+  <si>
+    <t>AUE1PRDIN02</t>
+  </si>
+  <si>
+    <t>10.210.1.111</t>
+  </si>
+  <si>
+    <t>AWSUE1DEVSA01</t>
+  </si>
+  <si>
+    <t>10.212.0.84</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2019 Datacenter  10.0.17763 Build 17763.3046</t>
+  </si>
+  <si>
+    <t>AWSUE1DEVSA02</t>
+  </si>
+  <si>
+    <t>10.212.0.112</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2019 Datacenter 10.0.17763 Build 17763.2928</t>
+  </si>
+  <si>
+    <t>AWSUE1QAAP01</t>
+  </si>
+  <si>
+    <t>10.211.0.101</t>
+  </si>
+  <si>
+    <t>AWSUE1QAAP02</t>
+  </si>
+  <si>
+    <t>10.211.1.101</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Server 2019 Datacenter 10.0.17763 Build 17763.3046</t>
+  </si>
+  <si>
+    <t>AWSUE1QAIN01</t>
+  </si>
+  <si>
+    <t>10.211.0.111</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>ACUSE1-LPAEC001</t>
+  </si>
+  <si>
+    <t>10.113.32.71</t>
+  </si>
+  <si>
+    <t>Other 3.x Linux (64-bit)</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Device Name</t>
+  </si>
+  <si>
+    <t>Device Model</t>
+  </si>
+  <si>
+    <t>Current VMware Version</t>
+  </si>
+  <si>
+    <t>Recommended Version</t>
+  </si>
+  <si>
+    <t>HyperFlex Version (if applicable)</t>
+  </si>
+  <si>
+    <t>HyperFlex Version Recommended</t>
+  </si>
+  <si>
+    <t>Server Hardware Firmware Version</t>
+  </si>
+  <si>
+    <t>Recommended Firmware</t>
   </si>
 </sst>
 </file>
@@ -315,6 +499,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>273797</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>100080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2102597" cy="481080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:M12" totalsRowCount="1">
   <autoFilter ref="A5:M11"/>
@@ -332,6 +559,25 @@
     <tableColumn id="11" name="Column11"/>
     <tableColumn id="12" name="Column12"/>
     <tableColumn id="13" name="Column13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:J24" totalsRowCount="1">
+  <autoFilter ref="A5:J23"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
+    <tableColumn id="10" name="Column10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -934,4 +1180,638 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:J3"/>
+    <mergeCell ref="A4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>